<commit_message>
CP01CNSP 00004 cal sheet update
Changed port numbers on reference designator to match reference
designator sheet, corrected lat lon format
</commit_message>
<xml_diff>
--- a/CP01CNSP/Omaha_Cal_Info_CP01CNSP_00004.xlsx
+++ b/CP01CNSP/Omaha_Cal_Info_CP01CNSP_00004.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="5900" windowWidth="31140" windowHeight="13800" tabRatio="579"/>
+    <workbookView xWindow="600" yWindow="5895" windowWidth="29040" windowHeight="13800" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
   <si>
     <t>Ref Des</t>
   </si>
@@ -282,28 +282,13 @@
     <t>CP01CNSP</t>
   </si>
   <si>
-    <t>CP01CNSP-SP001-02-DOSTAJ000</t>
-  </si>
-  <si>
     <t>Requires TEMPWAT, PRESWAT and PRACSAL from CP01CNSP-SP001-09-CTDPFJ000</t>
-  </si>
-  <si>
-    <t>CP01CNSP-SP001-04-OPTAAJ000</t>
   </si>
   <si>
     <t>CP01CNSP-SP001-05-VELPTJ000</t>
   </si>
   <si>
-    <t>CP01CNSP-SP001-06-NUTNRJ000</t>
-  </si>
-  <si>
     <t>CP01CNSP-SP001-07-SPKIRJ000</t>
-  </si>
-  <si>
-    <t>CP01CNSP-SP001-08-FLORTJ000</t>
-  </si>
-  <si>
-    <t>CP01CNSP-SP001-09-CTDPFJ000</t>
   </si>
   <si>
     <t>CP01CNSP-SP001-10-PARADJ000</t>
@@ -313,9 +298,6 @@
   </si>
   <si>
     <t>CP01CNSP-00004</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Ship: Scarlett Isabella (no cruise number)</t>
@@ -383,19 +365,43 @@
   <si>
     <t>[16, 27, 28, 29, 44, 43, 50, 48, 40, 43, 130, 380, 968, 2186, 4312, 7363, 11054, 14692, 17674, 19760, 21092, 21945, 22584, 23215, 23984, 24955, 26204, 27723, 29521, 31632, 33920, 36384, 38826, 41148, 43200, 44793, 45763, 46087, 45708, 44648, 43123, 41266, 39310, 37415, 35703, 34260, 33169, 32380, 31954, 31855, 32046, 32567, 33391, 34437, 35756, 37317, 39038, 40855, 42820, 44732, 46572, 48223, 49604, 50624, 51182, 51193, 50687, 49651, 48155, 46259, 44167, 41883, 39615, 37361, 35266, 33358, 31607, 30040, 28685, 27531, 26515, 25712, 25005, 24518, 24149, 23899, 23796, 23820, 23945, 24192, 24532, 24972, 25515, 26099, 26734, 27406, 28055, 28637, 29172, 29566, 29790, 29815, 29624, 29213, 28607, 27843, 26960, 25985, 24988, 23961, 23002, 22079, 21235, 20471, 19800, 19212, 18708, 18288, 17971, 17707, 17529, 17423, 17392, 17461, 17568, 17773, 18023, 18377, 18760, 19198, 19696, 20267, 20841, 21475, 22144, 22850, 23556, 24279, 24976, 25695, 26352, 26953, 27521, 28026, 28423, 28756, 28951, 29063, 29068, 28896, 28635, 28283, 27826, 27289, 26699, 26034, 25352, 24652, 23950, 23269, 22596, 21940, 21357, 20807, 20302, 19855, 19448, 19072, 18741, 18380, 18062, 17748, 17425, 17128, 16862, 16615, 16395, 16191, 16009, 15835, 15688, 15546, 15425, 15301, 15160, 15057, 14955, 14851, 14762, 14705, 14620, 14540, 14506, 14478, 14461, 14468, 14447, 14457, 14456, 14466, 14498, 14542, 14544, 14576, 14579, 14579, 14568, 14540, 14487, 14414, 14320, 14209, 14088, 13932, 13747, 13556, 13341, 13113, 12888, 12645, 12409, 12178, 11893, 11614, 11294, 10984, 10687, 10435, 10200, 9975, 9785, 9610, 9449, 9321, 9189, 9100, 9001, 8848, 8690, 8524, 8380, 8264, 8148, 8052, 7976, 7905, 7866, 7827, 7769, 7738, 7600, 7293, 6878, 6370, 5749, 4916]</t>
   </si>
+  <si>
+    <t>Scarlett Isabella</t>
+  </si>
+  <si>
+    <t>CP01CNSP-SP001-06-DOSTAJ000</t>
+  </si>
+  <si>
+    <t>CP01CNSP-SP001-02-OPTAAJ000</t>
+  </si>
+  <si>
+    <t>CP01CNSP-SP001-03-NUTNRJ000</t>
+  </si>
+  <si>
+    <t>CP01CNSP-SP001-09-FLORTJ000</t>
+  </si>
+  <si>
+    <t>CP01CNSP-SP001-08-CTDPFJ000</t>
+  </si>
+  <si>
+    <t>70°46.2'W</t>
+  </si>
+  <si>
+    <t>40°8.05'N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,6 +638,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -749,14 +761,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1324,7 +1336,7 @@
     <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1355,10 +1367,10 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1378,9 +1390,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="33" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1392,10 +1401,10 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1403,6 +1412,9 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="548">
@@ -1969,7 +1981,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -2313,28 +2325,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="39.5" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="12" customFormat="1" ht="28">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2369,124 +2381,124 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>42208</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="30"/>
-      <c r="G2" s="32">
-        <v>40.134083333333336</v>
-      </c>
-      <c r="H2" s="32">
-        <v>-70.770133333333305</v>
-      </c>
-      <c r="I2" s="40">
+      <c r="G2" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="39">
         <v>134</v>
       </c>
-      <c r="J2" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="40" t="s">
-        <v>78</v>
+      <c r="J2" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
     </row>
-    <row r="3" spans="1:13" s="21" customFormat="1">
+    <row r="3" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C3" s="22"/>
       <c r="D3" s="23"/>
       <c r="E3" s="24"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:13" s="21" customFormat="1">
+    <row r="4" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C4" s="22"/>
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:13" s="21" customFormat="1">
+    <row r="5" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C5" s="22"/>
       <c r="D5" s="23"/>
       <c r="E5" s="24"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:13" s="21" customFormat="1">
+    <row r="6" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C6" s="22"/>
       <c r="D6" s="23"/>
       <c r="E6" s="24"/>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:13" s="21" customFormat="1">
+    <row r="7" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C7" s="22"/>
       <c r="D7" s="23"/>
       <c r="E7" s="24"/>
       <c r="F7" s="23"/>
     </row>
-    <row r="8" spans="1:13" s="21" customFormat="1">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C8" s="22"/>
       <c r="D8" s="23"/>
       <c r="E8" s="24"/>
       <c r="F8" s="23"/>
     </row>
-    <row r="9" spans="1:13" s="21" customFormat="1">
+    <row r="9" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C9" s="22"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="1:13" s="21" customFormat="1">
+    <row r="10" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C10" s="22"/>
       <c r="D10" s="23"/>
       <c r="E10" s="24"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="1:13" s="21" customFormat="1">
+    <row r="11" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C11" s="22"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24"/>
       <c r="F11" s="23"/>
     </row>
-    <row r="12" spans="1:13" s="21" customFormat="1">
+    <row r="12" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C12" s="22"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
       <c r="F12" s="23"/>
     </row>
-    <row r="13" spans="1:13" s="21" customFormat="1">
+    <row r="13" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C13" s="22"/>
       <c r="D13" s="23"/>
       <c r="E13" s="24"/>
       <c r="F13" s="23"/>
     </row>
-    <row r="14" spans="1:13" s="21" customFormat="1">
+    <row r="14" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C14" s="22"/>
       <c r="D14" s="23"/>
       <c r="E14" s="24"/>
       <c r="F14" s="23"/>
     </row>
-    <row r="15" spans="1:13" s="21" customFormat="1">
+    <row r="15" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C15" s="22"/>
       <c r="D15" s="23"/>
       <c r="E15" s="24"/>
       <c r="F15" s="23"/>
     </row>
-    <row r="16" spans="1:13" s="21" customFormat="1">
+    <row r="16" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C16" s="22"/>
       <c r="D16" s="23"/>
       <c r="E16" s="24"/>
       <c r="F16" s="23"/>
     </row>
-    <row r="17" spans="3:6" s="21" customFormat="1">
+    <row r="17" spans="3:6" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
       <c r="E17" s="24"/>
@@ -2507,22 +2519,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.1640625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2545,924 +2557,924 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="13" customFormat="1">
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>76</v>
+        <v>95</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C3" s="26">
         <v>4</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="35">
         <v>351</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="40">
         <v>40.134083333333336</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="13" customFormat="1">
+    <row r="4" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>76</v>
+        <v>95</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C4" s="27">
         <v>4</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="35">
         <v>351</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="40">
         <v>-70.770133333333305</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="13" customFormat="1">
+    <row r="5" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>76</v>
+        <v>95</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="27">
         <v>4</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="35">
         <v>351</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>92</v>
+      <c r="F5" s="35" t="s">
+        <v>86</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="13" customFormat="1">
+    <row r="6" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
-      <c r="B6" s="34"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="27"/>
-      <c r="D6" s="36"/>
+      <c r="D6" s="35"/>
       <c r="F6" s="28"/>
     </row>
-    <row r="7" spans="1:7" s="13" customFormat="1">
+    <row r="7" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C7" s="26">
         <v>4</v>
       </c>
-      <c r="D7" s="37" t="s">
-        <v>80</v>
+      <c r="D7" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="36" t="s">
-        <v>85</v>
+      <c r="F7" s="35" t="s">
+        <v>79</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="13" customFormat="1">
+    <row r="8" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C8" s="27">
         <v>4</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>80</v>
+      <c r="D8" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="36" t="s">
-        <v>86</v>
+      <c r="F8" s="35" t="s">
+        <v>80</v>
       </c>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" s="13" customFormat="1">
+    <row r="9" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="27">
         <v>4</v>
       </c>
-      <c r="D9" s="37" t="s">
-        <v>80</v>
+      <c r="D9" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="35">
         <v>22</v>
       </c>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1">
+    <row r="10" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C10" s="27">
         <v>4</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>80</v>
+      <c r="D10" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="36" t="s">
-        <v>87</v>
+      <c r="F10" s="35" t="s">
+        <v>81</v>
       </c>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1">
+    <row r="11" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C11" s="27">
         <v>4</v>
       </c>
-      <c r="D11" s="37" t="s">
-        <v>80</v>
+      <c r="D11" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="36" t="s">
-        <v>88</v>
+      <c r="F11" s="35" t="s">
+        <v>82</v>
       </c>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1">
+    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C12" s="27">
         <v>4</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>80</v>
+      <c r="D12" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="36" t="s">
-        <v>90</v>
+      <c r="F12" s="35" t="s">
+        <v>84</v>
       </c>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1">
+    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C13" s="27">
         <v>4</v>
       </c>
-      <c r="D13" s="37" t="s">
-        <v>80</v>
+      <c r="D13" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="36" t="s">
-        <v>91</v>
+      <c r="F13" s="35" t="s">
+        <v>85</v>
       </c>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1">
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C14" s="27">
         <v>4</v>
       </c>
-      <c r="D14" s="37" t="s">
-        <v>80</v>
+      <c r="D14" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>89</v>
+      <c r="F14" s="35" t="s">
+        <v>83</v>
       </c>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1">
+    <row r="15" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
-      <c r="B15" s="34"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
       <c r="F15" s="28"/>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1">
+    <row r="16" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C16" s="26">
         <v>4</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>81</v>
+      <c r="D16" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="40">
         <v>40.134083333333336</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="13" customFormat="1">
+    <row r="17" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C17" s="27">
         <v>4</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>81</v>
+      <c r="D17" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="41">
+      <c r="F17" s="40">
         <v>-70.770133333333305</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1">
+    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
-      <c r="B18" s="34"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
       <c r="F18" s="28"/>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1">
+    <row r="19" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C19" s="26">
         <v>4</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="35">
         <v>428</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="42">
         <v>217</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1">
+    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C20" s="27">
         <v>4</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="35">
         <v>428</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="42">
         <v>240</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1">
+    <row r="21" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C21" s="27">
         <v>4</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="35">
         <v>428</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="35">
         <v>20</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1">
+    <row r="22" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C22" s="27">
         <v>4</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="35">
         <v>428</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="36" t="s">
-        <v>96</v>
+      <c r="F22" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="13" customFormat="1">
+    <row r="23" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C23" s="27">
         <v>4</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="35">
         <v>428</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="36" t="s">
-        <v>97</v>
+      <c r="F23" s="35" t="s">
+        <v>91</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="13" customFormat="1">
+    <row r="24" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C24" s="27">
         <v>4</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="35">
         <v>428</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="36" t="s">
-        <v>98</v>
+      <c r="F24" s="35" t="s">
+        <v>92</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="13" customFormat="1">
+    <row r="25" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>76</v>
+        <v>97</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C25" s="27">
         <v>4</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="35">
         <v>428</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="36" t="s">
-        <v>99</v>
+      <c r="F25" s="35" t="s">
+        <v>93</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="13" customFormat="1">
+    <row r="26" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
-      <c r="B26" s="34"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="27"/>
       <c r="D26" s="28"/>
       <c r="F26" s="28"/>
     </row>
-    <row r="27" spans="1:7" s="13" customFormat="1">
+    <row r="27" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="33" t="s">
         <v>71</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>76</v>
       </c>
       <c r="C27" s="26">
         <v>4</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D27" s="35">
         <v>265</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="36" t="s">
-        <v>93</v>
+      <c r="F27" s="35" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="13" customFormat="1">
+    <row r="28" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="33" t="s">
         <v>71</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>76</v>
       </c>
       <c r="C28" s="27">
         <v>4</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="35">
         <v>265</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="36" t="s">
-        <v>94</v>
+      <c r="F28" s="35" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="13" customFormat="1">
+    <row r="29" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="33" t="s">
         <v>71</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>76</v>
       </c>
       <c r="C29" s="27">
         <v>4</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="35">
         <v>265</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="36" t="s">
-        <v>95</v>
+      <c r="F29" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="13" customFormat="1">
+    <row r="30" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
-      <c r="B30" s="34"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
       <c r="F30" s="28"/>
     </row>
-    <row r="31" spans="1:7" s="13" customFormat="1">
+    <row r="31" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C31" s="26">
         <v>4</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="35">
         <v>1205</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="36">
+      <c r="F31" s="35">
         <v>49</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="13" customFormat="1">
+    <row r="32" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C32" s="27">
         <v>4</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="35">
         <v>1205</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="42">
+      <c r="F32" s="41">
         <v>3.0630000000000002E-6</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="13" customFormat="1">
+    <row r="33" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C33" s="27">
         <v>4</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D33" s="35">
         <v>1205</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="35">
         <v>46</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="13" customFormat="1">
+    <row r="34" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C34" s="27">
         <v>4</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="35">
         <v>1205</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="36">
+      <c r="F34" s="35">
         <v>1.21E-2</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="13" customFormat="1">
+    <row r="35" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C35" s="27">
         <v>4</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D35" s="35">
         <v>1205</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F35" s="35">
         <v>33</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="13" customFormat="1">
+    <row r="36" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C36" s="27">
         <v>4</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D36" s="35">
         <v>1205</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="36">
+      <c r="F36" s="35">
         <v>9.0300000000000005E-2</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="13" customFormat="1">
+    <row r="37" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C37" s="27">
         <v>4</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="35">
         <v>1205</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="43">
+      <c r="F37" s="42">
         <v>124</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="13" customFormat="1">
+    <row r="38" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C38" s="27">
         <v>4</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="35">
         <v>1205</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F38" s="43">
+      <c r="F38" s="42">
         <v>700</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="13" customFormat="1">
+    <row r="39" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C39" s="27">
         <v>4</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="35">
         <v>1205</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="43">
+      <c r="F39" s="42">
         <v>1.0760000000000001</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="13" customFormat="1">
+    <row r="40" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C40" s="27">
         <v>4</v>
       </c>
-      <c r="D40" s="36">
+      <c r="D40" s="35">
         <v>1205</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="43">
+      <c r="F40" s="42">
         <v>3.9E-2</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="13" customFormat="1">
+    <row r="41" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
-      <c r="B41" s="34"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
       <c r="F41" s="28"/>
     </row>
-    <row r="42" spans="1:7" s="13" customFormat="1">
+    <row r="42" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>76</v>
+        <v>99</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C42" s="26">
         <v>4</v>
       </c>
-      <c r="D42" s="36" t="s">
-        <v>82</v>
+      <c r="D42" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="41">
-        <v>40.134083333333336</v>
+      <c r="F42" s="40">
+        <v>40.134083333333301</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="13" customFormat="1">
+    <row r="43" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>76</v>
+        <v>99</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C43" s="27">
         <v>4</v>
       </c>
-      <c r="D43" s="36" t="s">
-        <v>82</v>
+      <c r="D43" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="41">
+      <c r="F43" s="40">
         <v>-70.770133333333305</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="13" customFormat="1">
+    <row r="44" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
-      <c r="B44" s="34"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="27"/>
       <c r="D44" s="28"/>
       <c r="F44" s="28"/>
     </row>
-    <row r="45" spans="1:7" s="13" customFormat="1">
+    <row r="45" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C45" s="26">
         <v>4</v>
       </c>
-      <c r="D45" s="36">
+      <c r="D45" s="35">
         <v>437</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="36">
+      <c r="F45" s="35">
         <v>1.3589</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="13" customFormat="1">
+    <row r="46" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C46" s="27">
         <v>4</v>
       </c>
-      <c r="D46" s="36">
+      <c r="D46" s="35">
         <v>437</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="36">
+      <c r="F46" s="35">
         <v>2903</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="13" customFormat="1">
+    <row r="47" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C47" s="27">
         <v>4</v>
       </c>
-      <c r="D47" s="36">
+      <c r="D47" s="35">
         <v>437</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F47" s="36">
+      <c r="F47" s="35">
         <v>3991</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="25" customFormat="1">
-      <c r="B48" s="35"/>
+    <row r="48" spans="1:7" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="34"/>
       <c r="C48" s="26"/>
       <c r="F48" s="29"/>
     </row>
-    <row r="49" spans="1:6" s="13" customFormat="1">
+    <row r="49" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C49" s="26">
         <v>4</v>
       </c>
-      <c r="D49" s="34" t="s">
-        <v>79</v>
+      <c r="D49" s="33" t="s">
+        <v>73</v>
       </c>
       <c r="F49" s="30"/>
     </row>
-    <row r="50" spans="1:6" s="13" customFormat="1"/>
-    <row r="51" spans="1:6" s="13" customFormat="1"/>
-    <row r="52" spans="1:6" s="13" customFormat="1"/>
-    <row r="53" spans="1:6" s="13" customFormat="1"/>
+    <row r="50" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3480,12 +3492,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5" style="33"/>
+    <col min="1" max="16384" width="11.42578125" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" customFormat="1">
+    <row r="1" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-0.133385</v>
       </c>
@@ -3598,7 +3610,7 @@
         <v>5.9284000000000003E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:37" customFormat="1">
+    <row r="2" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-0.12271600000000001</v>
       </c>
@@ -3711,7 +3723,7 @@
         <v>5.2031000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" customFormat="1">
+    <row r="3" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-0.106986</v>
       </c>
@@ -3824,7 +3836,7 @@
         <v>4.5156000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" customFormat="1">
+    <row r="4" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-9.3688999999999995E-2</v>
       </c>
@@ -3937,7 +3949,7 @@
         <v>3.7352999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" customFormat="1">
+    <row r="5" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-8.2291000000000003E-2</v>
       </c>
@@ -4050,7 +4062,7 @@
         <v>3.1369000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" customFormat="1">
+    <row r="6" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-7.1478E-2</v>
       </c>
@@ -4163,7 +4175,7 @@
         <v>2.6693999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" customFormat="1">
+    <row r="7" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-6.3391000000000003E-2</v>
       </c>
@@ -4276,7 +4288,7 @@
         <v>2.3102999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" customFormat="1">
+    <row r="8" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-5.6606999999999998E-2</v>
       </c>
@@ -4389,7 +4401,7 @@
         <v>2.0542000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" customFormat="1">
+    <row r="9" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-5.1151000000000002E-2</v>
       </c>
@@ -4502,7 +4514,7 @@
         <v>1.8499000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" customFormat="1">
+    <row r="10" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-4.6461000000000002E-2</v>
       </c>
@@ -4615,7 +4627,7 @@
         <v>1.6685999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" customFormat="1">
+    <row r="11" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-4.2729999999999997E-2</v>
       </c>
@@ -4728,7 +4740,7 @@
         <v>1.5391E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" customFormat="1">
+    <row r="12" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-3.9294000000000003E-2</v>
       </c>
@@ -4841,7 +4853,7 @@
         <v>1.3746E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:37" customFormat="1">
+    <row r="13" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-3.6886000000000002E-2</v>
       </c>
@@ -4954,7 +4966,7 @@
         <v>1.2531E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" customFormat="1">
+    <row r="14" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-3.4603000000000002E-2</v>
       </c>
@@ -5067,7 +5079,7 @@
         <v>1.1544E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:37" customFormat="1">
+    <row r="15" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-3.2263E-2</v>
       </c>
@@ -5180,7 +5192,7 @@
         <v>1.0629E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" customFormat="1">
+    <row r="16" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-3.0047999999999998E-2</v>
       </c>
@@ -5293,7 +5305,7 @@
         <v>9.9539999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37" customFormat="1">
+    <row r="17" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-2.8740000000000002E-2</v>
       </c>
@@ -5406,7 +5418,7 @@
         <v>9.3489999999999997E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37" customFormat="1">
+    <row r="18" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-2.6904000000000001E-2</v>
       </c>
@@ -5519,7 +5531,7 @@
         <v>8.8509999999999995E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" customFormat="1">
+    <row r="19" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-2.5165E-2</v>
       </c>
@@ -5632,7 +5644,7 @@
         <v>8.4279999999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37" customFormat="1">
+    <row r="20" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-2.3598999999999998E-2</v>
       </c>
@@ -5745,7 +5757,7 @@
         <v>8.0029999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" customFormat="1">
+    <row r="21" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-2.2419999999999999E-2</v>
       </c>
@@ -5858,7 +5870,7 @@
         <v>7.7739999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" customFormat="1">
+    <row r="22" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-2.1426000000000001E-2</v>
       </c>
@@ -5971,7 +5983,7 @@
         <v>7.5079999999999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:37" customFormat="1">
+    <row r="23" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-2.0347000000000001E-2</v>
       </c>
@@ -6084,7 +6096,7 @@
         <v>7.2659999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:37" customFormat="1">
+    <row r="24" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-1.9337E-2</v>
       </c>
@@ -6197,7 +6209,7 @@
         <v>6.9820000000000004E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" customFormat="1">
+    <row r="25" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1.8768E-2</v>
       </c>
@@ -6310,7 +6322,7 @@
         <v>6.8100000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:37" customFormat="1">
+    <row r="26" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-1.8110000000000001E-2</v>
       </c>
@@ -6423,7 +6435,7 @@
         <v>6.5440000000000003E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:37" customFormat="1">
+    <row r="27" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-1.7107000000000001E-2</v>
       </c>
@@ -6536,7 +6548,7 @@
         <v>6.3699999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:37" customFormat="1">
+    <row r="28" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-1.6622000000000001E-2</v>
       </c>
@@ -6649,7 +6661,7 @@
         <v>6.1609999999999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37" customFormat="1">
+    <row r="29" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-1.6263E-2</v>
       </c>
@@ -6762,7 +6774,7 @@
         <v>5.9849999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37" customFormat="1">
+    <row r="30" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-1.5591000000000001E-2</v>
       </c>
@@ -6875,7 +6887,7 @@
         <v>5.7970000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:37" customFormat="1">
+    <row r="31" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-1.5424999999999999E-2</v>
       </c>
@@ -6988,7 +7000,7 @@
         <v>5.6020000000000002E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37" customFormat="1">
+    <row r="32" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-1.4819000000000001E-2</v>
       </c>
@@ -7101,7 +7113,7 @@
         <v>5.4010000000000004E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37" customFormat="1">
+    <row r="33" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-1.4581E-2</v>
       </c>
@@ -7214,7 +7226,7 @@
         <v>5.1939999999999998E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37" customFormat="1">
+    <row r="34" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-1.4089000000000001E-2</v>
       </c>
@@ -7327,7 +7339,7 @@
         <v>4.9490000000000003E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:37" customFormat="1">
+    <row r="35" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1.3668E-2</v>
       </c>
@@ -7440,7 +7452,7 @@
         <v>4.7390000000000002E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:37" customFormat="1">
+    <row r="36" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-1.3519E-2</v>
       </c>
@@ -7553,7 +7565,7 @@
         <v>4.4320000000000002E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37" customFormat="1">
+    <row r="37" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-1.3158E-2</v>
       </c>
@@ -7666,7 +7678,7 @@
         <v>4.1269999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:37" customFormat="1">
+    <row r="38" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-1.3108E-2</v>
       </c>
@@ -7779,7 +7791,7 @@
         <v>3.7820000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:37" customFormat="1">
+    <row r="39" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-1.3062000000000001E-2</v>
       </c>
@@ -7892,7 +7904,7 @@
         <v>3.4949999999999998E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37" customFormat="1">
+    <row r="40" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-1.3098E-2</v>
       </c>
@@ -8005,7 +8017,7 @@
         <v>3.1670000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:37" customFormat="1">
+    <row r="41" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-1.2859000000000001E-2</v>
       </c>
@@ -8118,7 +8130,7 @@
         <v>2.947E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37" customFormat="1">
+    <row r="42" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-1.281E-2</v>
       </c>
@@ -8231,7 +8243,7 @@
         <v>2.686E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37" customFormat="1">
+    <row r="43" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-1.2343E-2</v>
       </c>
@@ -8344,7 +8356,7 @@
         <v>2.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" customFormat="1">
+    <row r="44" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-1.1986999999999999E-2</v>
       </c>
@@ -8457,7 +8469,7 @@
         <v>2.3860000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:37" customFormat="1">
+    <row r="45" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-1.0781000000000001E-2</v>
       </c>
@@ -8570,7 +8582,7 @@
         <v>3.2550000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" customFormat="1">
+    <row r="46" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-1.073E-2</v>
       </c>
@@ -8683,7 +8695,7 @@
         <v>3.2039999999999998E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37" customFormat="1">
+    <row r="47" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-1.0609E-2</v>
       </c>
@@ -8796,7 +8808,7 @@
         <v>3.1679999999999998E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37" customFormat="1">
+    <row r="48" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-1.0292000000000001E-2</v>
       </c>
@@ -8909,7 +8921,7 @@
         <v>3.2160000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:37" customFormat="1">
+    <row r="49" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-1.0172E-2</v>
       </c>
@@ -9022,7 +9034,7 @@
         <v>3.1280000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37" customFormat="1">
+    <row r="50" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-1.0064999999999999E-2</v>
       </c>
@@ -9135,7 +9147,7 @@
         <v>3.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37" customFormat="1">
+    <row r="51" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-1.0063000000000001E-2</v>
       </c>
@@ -9248,7 +9260,7 @@
         <v>3.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37" customFormat="1">
+    <row r="52" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-9.9609999999999994E-3</v>
       </c>
@@ -9361,7 +9373,7 @@
         <v>3.228E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37" customFormat="1">
+    <row r="53" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-9.9220000000000003E-3</v>
       </c>
@@ -9474,7 +9486,7 @@
         <v>3.2469999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:37" customFormat="1">
+    <row r="54" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-9.9830000000000006E-3</v>
       </c>
@@ -9587,7 +9599,7 @@
         <v>3.228E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37" customFormat="1">
+    <row r="55" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-9.9399999999999992E-3</v>
       </c>
@@ -9700,7 +9712,7 @@
         <v>3.238E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37" customFormat="1">
+    <row r="56" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-9.9799999999999993E-3</v>
       </c>
@@ -9813,7 +9825,7 @@
         <v>3.212E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37" customFormat="1">
+    <row r="57" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-1.005E-2</v>
       </c>
@@ -9926,7 +9938,7 @@
         <v>3.2620000000000001E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37" customFormat="1">
+    <row r="58" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-1.0281999999999999E-2</v>
       </c>
@@ -10039,7 +10051,7 @@
         <v>3.1909999999999998E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37" customFormat="1">
+    <row r="59" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-1.0265E-2</v>
       </c>
@@ -10152,7 +10164,7 @@
         <v>3.2139999999999998E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:37" customFormat="1">
+    <row r="60" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-1.0356000000000001E-2</v>
       </c>
@@ -10265,7 +10277,7 @@
         <v>3.1649999999999998E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37" customFormat="1">
+    <row r="61" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-1.0489999999999999E-2</v>
       </c>
@@ -10378,7 +10390,7 @@
         <v>3.1199999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37" customFormat="1">
+    <row r="62" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-1.0866000000000001E-2</v>
       </c>
@@ -10491,7 +10503,7 @@
         <v>3.1120000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37" customFormat="1">
+    <row r="63" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-1.0864E-2</v>
       </c>
@@ -10604,7 +10616,7 @@
         <v>3.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37" customFormat="1">
+    <row r="64" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-1.0709E-2</v>
       </c>
@@ -10717,7 +10729,7 @@
         <v>2.9120000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" customFormat="1">
+    <row r="65" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-1.0669E-2</v>
       </c>
@@ -10830,7 +10842,7 @@
         <v>2.8289999999999999E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:37" customFormat="1">
+    <row r="66" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-1.0749999999999999E-2</v>
       </c>
@@ -10943,7 +10955,7 @@
         <v>2.6580000000000002E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37" customFormat="1">
+    <row r="67" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-1.0749999999999999E-2</v>
       </c>
@@ -11056,7 +11068,7 @@
         <v>2.4369999999999999E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37" customFormat="1">
+    <row r="68" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-1.0692E-2</v>
       </c>
@@ -11169,7 +11181,7 @@
         <v>2.1849999999999999E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37" customFormat="1">
+    <row r="69" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-1.0525E-2</v>
       </c>
@@ -11282,7 +11294,7 @@
         <v>1.92E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37" customFormat="1">
+    <row r="70" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-1.0342E-2</v>
       </c>
@@ -11395,7 +11407,7 @@
         <v>1.655E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37" customFormat="1">
+    <row r="71" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-1.0305E-2</v>
       </c>
@@ -11508,7 +11520,7 @@
         <v>1.426E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37" customFormat="1">
+    <row r="72" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-1.0305999999999999E-2</v>
       </c>
@@ -11621,7 +11633,7 @@
         <v>1.3159999999999999E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" customFormat="1">
+    <row r="73" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-1.0312E-2</v>
       </c>
@@ -11734,7 +11746,7 @@
         <v>1.2030000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37" customFormat="1">
+    <row r="74" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-1.042E-2</v>
       </c>
@@ -11847,7 +11859,7 @@
         <v>1.2110000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:37" customFormat="1">
+    <row r="75" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-1.0284E-2</v>
       </c>
@@ -11960,7 +11972,7 @@
         <v>1.2030000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37" customFormat="1">
+    <row r="76" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-1.0463999999999999E-2</v>
       </c>
@@ -12073,7 +12085,7 @@
         <v>1.3470000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37" customFormat="1">
+    <row r="77" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-1.0571000000000001E-2</v>
       </c>
@@ -12186,7 +12198,7 @@
         <v>1.4829999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" customFormat="1">
+    <row r="78" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-1.0709E-2</v>
       </c>
@@ -12299,7 +12311,7 @@
         <v>1.578E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" customFormat="1">
+    <row r="79" spans="1:37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-1.0803E-2</v>
       </c>
@@ -12430,12 +12442,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5" style="13"/>
+    <col min="1" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="13">
         <v>-1.7871999999999999E-2</v>
       </c>
@@ -12548,7 +12560,7 @@
         <v>9.5980000000000006E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>-1.8088E-2</v>
       </c>
@@ -12661,7 +12673,7 @@
         <v>4.3020000000000003E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>-1.7731E-2</v>
       </c>
@@ -12774,7 +12786,7 @@
         <v>7.8580000000000004E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>-1.8546E-2</v>
       </c>
@@ -12887,7 +12899,7 @@
         <v>7.7479999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>-1.8301999999999999E-2</v>
       </c>
@@ -13000,7 +13012,7 @@
         <v>8.0269999999999994E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>-1.8294999999999999E-2</v>
       </c>
@@ -13113,7 +13125,7 @@
         <v>7.4859999999999996E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>-2.0648E-2</v>
       </c>
@@ -13226,7 +13238,7 @@
         <v>6.5230000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>-2.027E-2</v>
       </c>
@@ -13339,7 +13351,7 @@
         <v>6.4780000000000003E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>-1.7846000000000001E-2</v>
       </c>
@@ -13452,7 +13464,7 @@
         <v>7.4660000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>-1.4449999999999999E-2</v>
       </c>
@@ -13565,7 +13577,7 @@
         <v>8.2150000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>-1.5069000000000001E-2</v>
       </c>
@@ -13678,7 +13690,7 @@
         <v>7.6829999999999997E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>-1.6958999999999998E-2</v>
       </c>
@@ -13791,7 +13803,7 @@
         <v>6.398E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>-1.8593999999999999E-2</v>
       </c>
@@ -13904,7 +13916,7 @@
         <v>4.7869999999999996E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>-1.7714000000000001E-2</v>
       </c>
@@ -14017,7 +14029,7 @@
         <v>5.0980000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>-1.4026E-2</v>
       </c>
@@ -14130,7 +14142,7 @@
         <v>6.4669999999999997E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>-1.0862999999999999E-2</v>
       </c>
@@ -14243,7 +14255,7 @@
         <v>7.0780000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>-1.1547999999999999E-2</v>
       </c>
@@ -14356,7 +14368,7 @@
         <v>5.8129999999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>-1.3995E-2</v>
       </c>
@@ -14469,7 +14481,7 @@
         <v>3.741E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>-1.5415999999999999E-2</v>
       </c>
@@ -14582,7 +14594,7 @@
         <v>2.4989999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>-1.302E-2</v>
       </c>
@@ -14695,7 +14707,7 @@
         <v>3.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>-9.7009999999999996E-3</v>
       </c>
@@ -14808,7 +14820,7 @@
         <v>4.8830000000000002E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>-5.5519999999999996E-3</v>
       </c>
@@ -14921,7 +14933,7 @@
         <v>5.7920000000000003E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>-6.1029999999999999E-3</v>
       </c>
@@ -15034,7 +15046,7 @@
         <v>4.8349999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>-9.4459999999999995E-3</v>
       </c>
@@ -15147,7 +15159,7 @@
         <v>2.7230000000000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>-1.1916E-2</v>
       </c>
@@ -15260,7 +15272,7 @@
         <v>9.0600000000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>-1.162E-2</v>
       </c>
@@ -15373,7 +15385,7 @@
         <v>9.68E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>-8.2749999999999994E-3</v>
       </c>
@@ -15486,7 +15498,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>-4.0740000000000004E-3</v>
       </c>
@@ -15599,7 +15611,7 @@
         <v>4.5069999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>-1.5449999999999999E-3</v>
       </c>
@@ -15712,7 +15724,7 @@
         <v>5.0889999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>-2.8300000000000001E-3</v>
       </c>
@@ -15825,7 +15837,7 @@
         <v>3.6410000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>-6.313E-3</v>
       </c>
@@ -15938,7 +15950,7 @@
         <v>1.1379999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>-8.8730000000000007E-3</v>
       </c>
@@ -16051,7 +16063,7 @@
         <v>-4.6299999999999998E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>-8.6660000000000001E-3</v>
       </c>
@@ -16164,7 +16176,7 @@
         <v>-4.95E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>-5.4660000000000004E-3</v>
       </c>
@@ -16277,7 +16289,7 @@
         <v>9.8200000000000002E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>-6.2100000000000002E-4</v>
       </c>
@@ -16390,7 +16402,7 @@
         <v>3.1280000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>2.892E-3</v>
       </c>
@@ -16503,7 +16515,7 @@
         <v>4.2469999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>3.722E-3</v>
       </c>
@@ -16616,7 +16628,7 @@
         <v>3.9699999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>1.487E-3</v>
       </c>
@@ -16729,7 +16741,7 @@
         <v>2.3259999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>-1.918E-3</v>
       </c>
@@ -16842,7 +16854,7 @@
         <v>-1.9000000000000001E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>-4.9290000000000002E-3</v>
       </c>
@@ -16955,7 +16967,7 @@
         <v>-1.72E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>-5.9439999999999996E-3</v>
       </c>
@@ -17068,7 +17080,7 @@
         <v>-2.2699999999999999E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>-4.3629999999999997E-3</v>
       </c>
@@ -17181,7 +17193,7 @@
         <v>-1.4679999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>-9.0600000000000001E-4</v>
       </c>
@@ -17294,7 +17306,7 @@
         <v>4.2499999999999998E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>2.9910000000000002E-3</v>
       </c>
@@ -17407,7 +17419,7 @@
         <v>2.31E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>4.7140000000000003E-3</v>
       </c>
@@ -17520,7 +17532,7 @@
         <v>3.395E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>5.8609999999999999E-3</v>
       </c>
@@ -17633,7 +17645,7 @@
         <v>3.656E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>4.8219999999999999E-3</v>
       </c>
@@ -17746,7 +17758,7 @@
         <v>2.7009999999999998E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>1.977E-3</v>
       </c>
@@ -17859,7 +17871,7 @@
         <v>8.03E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>-1.575E-3</v>
       </c>
@@ -17972,7 +17984,7 @@
         <v>-1.1659999999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>-4.2989999999999999E-3</v>
       </c>
@@ -18085,7 +18097,7 @@
         <v>-2.6329999999999999E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>-5.1079999999999997E-3</v>
       </c>
@@ -18198,7 +18210,7 @@
         <v>-2.967E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>-3.8509999999999998E-3</v>
       </c>
@@ -18311,7 +18323,7 @@
         <v>-2.0950000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>-1.008E-3</v>
       </c>
@@ -18424,7 +18436,7 @@
         <v>-4.5399999999999998E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>2.6949999999999999E-3</v>
       </c>
@@ -18537,7 +18549,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>5.9519999999999998E-3</v>
       </c>
@@ -18650,7 +18662,7 @@
         <v>3.0739999999999999E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>7.9100000000000004E-3</v>
       </c>
@@ -18763,7 +18775,7 @@
         <v>3.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>7.7559999999999999E-3</v>
       </c>
@@ -18876,7 +18888,7 @@
         <v>3.5839999999999999E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>6.0660000000000002E-3</v>
       </c>
@@ -18989,7 +19001,7 @@
         <v>2.3960000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>3.14E-3</v>
       </c>
@@ -19102,7 +19114,7 @@
         <v>6.3100000000000005E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>1.3200000000000001E-4</v>
       </c>
@@ -19215,7 +19227,7 @@
         <v>-1.075E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>-2.2959999999999999E-3</v>
       </c>
@@ -19328,7 +19340,7 @@
         <v>-2.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>-3.689E-3</v>
       </c>
@@ -19441,7 +19453,7 @@
         <v>-2.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>-3.5109999999999998E-3</v>
       </c>
@@ -19554,7 +19566,7 @@
         <v>-2.5010000000000002E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>-1.6869999999999999E-3</v>
       </c>
@@ -19667,7 +19679,7 @@
         <v>-1.4090000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>9.01E-4</v>
       </c>
@@ -19780,7 +19792,7 @@
         <v>3.4999999999999997E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
         <v>3.9820000000000003E-3</v>
       </c>
@@ -19893,7 +19905,7 @@
         <v>1.7949999999999999E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>7.1980000000000004E-3</v>
       </c>
@@ -20006,7 +20018,7 @@
         <v>3.2130000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>8.8610000000000008E-3</v>
       </c>
@@ -20119,7 +20131,7 @@
         <v>4.1510000000000002E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>1.0116999999999999E-2</v>
       </c>
@@ -20232,7 +20244,7 @@
         <v>4.3810000000000003E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>9.9889999999999996E-3</v>
       </c>
@@ -20345,7 +20357,7 @@
         <v>4.0749999999999996E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>8.7559999999999999E-3</v>
       </c>
@@ -20458,7 +20470,7 @@
         <v>3.13E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>7.2090000000000001E-3</v>
       </c>
@@ -20571,7 +20583,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>4.4799999999999996E-3</v>
       </c>
@@ -20684,7 +20696,7 @@
         <v>3.3500000000000001E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:37">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>1.864E-3</v>
       </c>
@@ -20797,7 +20809,7 @@
         <v>-9.5600000000000004E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
         <v>2.3699999999999999E-4</v>
       </c>
@@ -20910,7 +20922,7 @@
         <v>-1.952E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" s="13">
         <v>-1.8400000000000001E-3</v>
       </c>
@@ -21023,7 +21035,7 @@
         <v>-2.8530000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
         <v>-2.4559999999999998E-3</v>
       </c>
@@ -21136,7 +21148,7 @@
         <v>-3.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
         <v>-2.1870000000000001E-3</v>
       </c>
@@ -21249,7 +21261,7 @@
         <v>-3.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" s="13">
         <v>-2.7109999999999999E-3</v>
       </c>
@@ -21380,35 +21392,35 @@
       <selection activeCell="A83" sqref="A83:XFD170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="58" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="70" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="78" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="58" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="70" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="78" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-0.133385</v>
       </c>
@@ -21521,7 +21533,7 @@
         <v>5.9284000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-0.12271600000000001</v>
       </c>
@@ -21634,7 +21646,7 @@
         <v>5.2031000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-0.106986</v>
       </c>
@@ -21747,7 +21759,7 @@
         <v>4.5156000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-9.3688999999999995E-2</v>
       </c>
@@ -21860,7 +21872,7 @@
         <v>3.7352999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-8.2291000000000003E-2</v>
       </c>
@@ -21973,7 +21985,7 @@
         <v>3.1369000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-7.1478E-2</v>
       </c>
@@ -22086,7 +22098,7 @@
         <v>2.6693999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-6.3391000000000003E-2</v>
       </c>
@@ -22199,7 +22211,7 @@
         <v>2.3102999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-5.6606999999999998E-2</v>
       </c>
@@ -22312,7 +22324,7 @@
         <v>2.0542000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-5.1151000000000002E-2</v>
       </c>
@@ -22425,7 +22437,7 @@
         <v>1.8499000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-4.6461000000000002E-2</v>
       </c>
@@ -22538,7 +22550,7 @@
         <v>1.6685999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-4.2729999999999997E-2</v>
       </c>
@@ -22651,7 +22663,7 @@
         <v>1.5391E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-3.9294000000000003E-2</v>
       </c>
@@ -22764,7 +22776,7 @@
         <v>1.3746E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-3.6886000000000002E-2</v>
       </c>
@@ -22877,7 +22889,7 @@
         <v>1.2531E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-3.4603000000000002E-2</v>
       </c>
@@ -22990,7 +23002,7 @@
         <v>1.1544E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-3.2263E-2</v>
       </c>
@@ -23103,7 +23115,7 @@
         <v>1.0629E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-3.0047999999999998E-2</v>
       </c>
@@ -23216,7 +23228,7 @@
         <v>9.9539999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-2.8740000000000002E-2</v>
       </c>
@@ -23329,7 +23341,7 @@
         <v>9.3489999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-2.6904000000000001E-2</v>
       </c>
@@ -23442,7 +23454,7 @@
         <v>8.8509999999999995E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-2.5165E-2</v>
       </c>
@@ -23555,7 +23567,7 @@
         <v>8.4279999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-2.3598999999999998E-2</v>
       </c>
@@ -23668,7 +23680,7 @@
         <v>8.0029999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-2.2419999999999999E-2</v>
       </c>
@@ -23781,7 +23793,7 @@
         <v>7.7739999999999997E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-2.1426000000000001E-2</v>
       </c>
@@ -23894,7 +23906,7 @@
         <v>7.5079999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-2.0347000000000001E-2</v>
       </c>
@@ -24007,7 +24019,7 @@
         <v>7.2659999999999999E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1.9337E-2</v>
       </c>
@@ -24120,7 +24132,7 @@
         <v>6.9820000000000004E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-1.8768E-2</v>
       </c>
@@ -24233,7 +24245,7 @@
         <v>6.8100000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-1.8110000000000001E-2</v>
       </c>
@@ -24346,7 +24358,7 @@
         <v>6.5440000000000003E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-1.7107000000000001E-2</v>
       </c>
@@ -24459,7 +24471,7 @@
         <v>6.3699999999999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-1.6622000000000001E-2</v>
       </c>
@@ -24572,7 +24584,7 @@
         <v>6.1609999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-1.6263E-2</v>
       </c>
@@ -24685,7 +24697,7 @@
         <v>5.9849999999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-1.5591000000000001E-2</v>
       </c>
@@ -24798,7 +24810,7 @@
         <v>5.7970000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-1.5424999999999999E-2</v>
       </c>
@@ -24911,7 +24923,7 @@
         <v>5.6020000000000002E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-1.4819000000000001E-2</v>
       </c>
@@ -25024,7 +25036,7 @@
         <v>5.4010000000000004E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-1.4581E-2</v>
       </c>
@@ -25137,7 +25149,7 @@
         <v>5.1939999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1.4089000000000001E-2</v>
       </c>
@@ -25250,7 +25262,7 @@
         <v>4.9490000000000003E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-1.3668E-2</v>
       </c>
@@ -25363,7 +25375,7 @@
         <v>4.7390000000000002E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-1.3519E-2</v>
       </c>
@@ -25476,7 +25488,7 @@
         <v>4.4320000000000002E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-1.3158E-2</v>
       </c>
@@ -25589,7 +25601,7 @@
         <v>4.1269999999999996E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-1.3108E-2</v>
       </c>
@@ -25702,7 +25714,7 @@
         <v>3.7820000000000002E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-1.3062000000000001E-2</v>
       </c>
@@ -25815,7 +25827,7 @@
         <v>3.4949999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-1.3098E-2</v>
       </c>
@@ -25928,7 +25940,7 @@
         <v>3.1670000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-1.2859000000000001E-2</v>
       </c>
@@ -26041,7 +26053,7 @@
         <v>2.947E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-1.281E-2</v>
       </c>
@@ -26154,7 +26166,7 @@
         <v>2.686E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-1.2343E-2</v>
       </c>
@@ -26267,7 +26279,7 @@
         <v>2.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-1.1986999999999999E-2</v>
       </c>
@@ -26380,7 +26392,7 @@
         <v>2.3860000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-1.0781000000000001E-2</v>
       </c>
@@ -26493,7 +26505,7 @@
         <v>3.2550000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-1.073E-2</v>
       </c>
@@ -26606,7 +26618,7 @@
         <v>3.2039999999999998E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-1.0609E-2</v>
       </c>
@@ -26719,7 +26731,7 @@
         <v>3.1679999999999998E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-1.0292000000000001E-2</v>
       </c>
@@ -26832,7 +26844,7 @@
         <v>3.2160000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-1.0172E-2</v>
       </c>
@@ -26945,7 +26957,7 @@
         <v>3.1280000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-1.0064999999999999E-2</v>
       </c>
@@ -27058,7 +27070,7 @@
         <v>3.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-1.0063000000000001E-2</v>
       </c>
@@ -27171,7 +27183,7 @@
         <v>3.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-9.9609999999999994E-3</v>
       </c>
@@ -27284,7 +27296,7 @@
         <v>3.228E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-9.9220000000000003E-3</v>
       </c>
@@ -27397,7 +27409,7 @@
         <v>3.2469999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-9.9830000000000006E-3</v>
       </c>
@@ -27510,7 +27522,7 @@
         <v>3.228E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-9.9399999999999992E-3</v>
       </c>
@@ -27623,7 +27635,7 @@
         <v>3.238E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-9.9799999999999993E-3</v>
       </c>
@@ -27736,7 +27748,7 @@
         <v>3.212E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-1.005E-2</v>
       </c>
@@ -27849,7 +27861,7 @@
         <v>3.2620000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-1.0281999999999999E-2</v>
       </c>
@@ -27962,7 +27974,7 @@
         <v>3.1909999999999998E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-1.0265E-2</v>
       </c>
@@ -28075,7 +28087,7 @@
         <v>3.2139999999999998E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-1.0356000000000001E-2</v>
       </c>
@@ -28188,7 +28200,7 @@
         <v>3.1649999999999998E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-1.0489999999999999E-2</v>
       </c>
@@ -28301,7 +28313,7 @@
         <v>3.1199999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-1.0866000000000001E-2</v>
       </c>
@@ -28414,7 +28426,7 @@
         <v>3.1120000000000002E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-1.0864E-2</v>
       </c>
@@ -28527,7 +28539,7 @@
         <v>3.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-1.0709E-2</v>
       </c>
@@ -28640,7 +28652,7 @@
         <v>2.9120000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-1.0669E-2</v>
       </c>
@@ -28753,7 +28765,7 @@
         <v>2.8289999999999999E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-1.0749999999999999E-2</v>
       </c>
@@ -28866,7 +28878,7 @@
         <v>2.6580000000000002E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-1.0749999999999999E-2</v>
       </c>
@@ -28979,7 +28991,7 @@
         <v>2.4369999999999999E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-1.0692E-2</v>
       </c>
@@ -29092,7 +29104,7 @@
         <v>2.1849999999999999E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-1.0525E-2</v>
       </c>
@@ -29205,7 +29217,7 @@
         <v>1.92E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-1.0342E-2</v>
       </c>
@@ -29318,7 +29330,7 @@
         <v>1.655E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-1.0305E-2</v>
       </c>
@@ -29431,7 +29443,7 @@
         <v>1.426E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-1.0305999999999999E-2</v>
       </c>
@@ -29544,7 +29556,7 @@
         <v>1.3159999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-1.0312E-2</v>
       </c>
@@ -29657,7 +29669,7 @@
         <v>1.2030000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-1.042E-2</v>
       </c>
@@ -29770,7 +29782,7 @@
         <v>1.2110000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-1.0284E-2</v>
       </c>
@@ -29883,7 +29895,7 @@
         <v>1.2030000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-1.0463999999999999E-2</v>
       </c>
@@ -29996,7 +30008,7 @@
         <v>1.3470000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-1.0571000000000001E-2</v>
       </c>
@@ -30109,7 +30121,7 @@
         <v>1.4829999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-1.0709E-2</v>
       </c>
@@ -30222,7 +30234,7 @@
         <v>1.578E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:37">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-1.0803E-2</v>
       </c>
@@ -30335,12 +30347,12 @@
         <v>1.622E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:37">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:37">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-1.7871999999999999E-2</v>
       </c>
@@ -30453,7 +30465,7 @@
         <v>9.5980000000000006E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:37">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-1.8088E-2</v>
       </c>
@@ -30566,7 +30578,7 @@
         <v>4.3020000000000003E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:37">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-1.7731E-2</v>
       </c>
@@ -30679,7 +30691,7 @@
         <v>7.8580000000000004E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:37">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>-1.8546E-2</v>
       </c>
@@ -30792,7 +30804,7 @@
         <v>7.7479999999999997E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:37">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>-1.8301999999999999E-2</v>
       </c>
@@ -30905,7 +30917,7 @@
         <v>8.0269999999999994E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:37">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>-1.8294999999999999E-2</v>
       </c>
@@ -31018,7 +31030,7 @@
         <v>7.4859999999999996E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:37">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>-2.0648E-2</v>
       </c>
@@ -31131,7 +31143,7 @@
         <v>6.5230000000000002E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:37">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>-2.027E-2</v>
       </c>
@@ -31244,7 +31256,7 @@
         <v>6.4780000000000003E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:37">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>-1.7846000000000001E-2</v>
       </c>
@@ -31357,7 +31369,7 @@
         <v>7.4660000000000004E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:37">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>-1.4449999999999999E-2</v>
       </c>
@@ -31470,7 +31482,7 @@
         <v>8.2150000000000001E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:37">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>-1.5069000000000001E-2</v>
       </c>
@@ -31583,7 +31595,7 @@
         <v>7.6829999999999997E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:37">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>-1.6958999999999998E-2</v>
       </c>
@@ -31696,7 +31708,7 @@
         <v>6.398E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:37">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>-1.8593999999999999E-2</v>
       </c>
@@ -31809,7 +31821,7 @@
         <v>4.7869999999999996E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:37">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>-1.7714000000000001E-2</v>
       </c>
@@ -31922,7 +31934,7 @@
         <v>5.0980000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:37">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>-1.4026E-2</v>
       </c>
@@ -32035,7 +32047,7 @@
         <v>6.4669999999999997E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:37">
+    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>-1.0862999999999999E-2</v>
       </c>
@@ -32148,7 +32160,7 @@
         <v>7.0780000000000001E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:37">
+    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>-1.1547999999999999E-2</v>
       </c>
@@ -32261,7 +32273,7 @@
         <v>5.8129999999999996E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:37">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>-1.3995E-2</v>
       </c>
@@ -32374,7 +32386,7 @@
         <v>3.741E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:37">
+    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>-1.5415999999999999E-2</v>
       </c>
@@ -32487,7 +32499,7 @@
         <v>2.4989999999999999E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:37">
+    <row r="102" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>-1.302E-2</v>
       </c>
@@ -32600,7 +32612,7 @@
         <v>3.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:37">
+    <row r="103" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>-9.7009999999999996E-3</v>
       </c>
@@ -32713,7 +32725,7 @@
         <v>4.8830000000000002E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:37">
+    <row r="104" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>-5.5519999999999996E-3</v>
       </c>
@@ -32826,7 +32838,7 @@
         <v>5.7920000000000003E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:37">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>-6.1029999999999999E-3</v>
       </c>
@@ -32939,7 +32951,7 @@
         <v>4.8349999999999999E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:37">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>-9.4459999999999995E-3</v>
       </c>
@@ -33052,7 +33064,7 @@
         <v>2.7230000000000002E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:37">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>-1.1916E-2</v>
       </c>
@@ -33165,7 +33177,7 @@
         <v>9.0600000000000001E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:37">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>-1.162E-2</v>
       </c>
@@ -33278,7 +33290,7 @@
         <v>9.68E-4</v>
       </c>
     </row>
-    <row r="109" spans="1:37">
+    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>-8.2749999999999994E-3</v>
       </c>
@@ -33391,7 +33403,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:37">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>-4.0740000000000004E-3</v>
       </c>
@@ -33504,7 +33516,7 @@
         <v>4.5069999999999997E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:37">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>-1.5449999999999999E-3</v>
       </c>
@@ -33617,7 +33629,7 @@
         <v>5.0889999999999998E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:37">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>-2.8300000000000001E-3</v>
       </c>
@@ -33730,7 +33742,7 @@
         <v>3.6410000000000001E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:37">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>-6.313E-3</v>
       </c>
@@ -33843,7 +33855,7 @@
         <v>1.1379999999999999E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:37">
+    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>-8.8730000000000007E-3</v>
       </c>
@@ -33956,7 +33968,7 @@
         <v>-4.6299999999999998E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:37">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>-8.6660000000000001E-3</v>
       </c>
@@ -34069,7 +34081,7 @@
         <v>-4.95E-4</v>
       </c>
     </row>
-    <row r="116" spans="1:37">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>-5.4660000000000004E-3</v>
       </c>
@@ -34182,7 +34194,7 @@
         <v>9.8200000000000002E-4</v>
       </c>
     </row>
-    <row r="117" spans="1:37">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>-6.2100000000000002E-4</v>
       </c>
@@ -34295,7 +34307,7 @@
         <v>3.1280000000000001E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:37">
+    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2.892E-3</v>
       </c>
@@ -34408,7 +34420,7 @@
         <v>4.2469999999999999E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:37">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>3.722E-3</v>
       </c>
@@ -34521,7 +34533,7 @@
         <v>3.9699999999999996E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:37">
+    <row r="120" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1.487E-3</v>
       </c>
@@ -34634,7 +34646,7 @@
         <v>2.3259999999999999E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:37">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>-1.918E-3</v>
       </c>
@@ -34747,7 +34759,7 @@
         <v>-1.9000000000000001E-5</v>
       </c>
     </row>
-    <row r="122" spans="1:37">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>-4.9290000000000002E-3</v>
       </c>
@@ -34860,7 +34872,7 @@
         <v>-1.72E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:37">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>-5.9439999999999996E-3</v>
       </c>
@@ -34973,7 +34985,7 @@
         <v>-2.2699999999999999E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:37">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>-4.3629999999999997E-3</v>
       </c>
@@ -35086,7 +35098,7 @@
         <v>-1.4679999999999999E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:37">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>-9.0600000000000001E-4</v>
       </c>
@@ -35199,7 +35211,7 @@
         <v>4.2499999999999998E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:37">
+    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2.9910000000000002E-3</v>
       </c>
@@ -35312,7 +35324,7 @@
         <v>2.31E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:37">
+    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>4.7140000000000003E-3</v>
       </c>
@@ -35425,7 +35437,7 @@
         <v>3.395E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:37">
+    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>5.8609999999999999E-3</v>
       </c>
@@ -35538,7 +35550,7 @@
         <v>3.656E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:37">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>4.8219999999999999E-3</v>
       </c>
@@ -35651,7 +35663,7 @@
         <v>2.7009999999999998E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:37">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1.977E-3</v>
       </c>
@@ -35764,7 +35776,7 @@
         <v>8.03E-4</v>
       </c>
     </row>
-    <row r="131" spans="1:37">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>-1.575E-3</v>
       </c>
@@ -35877,7 +35889,7 @@
         <v>-1.1659999999999999E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:37">
+    <row r="132" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>-4.2989999999999999E-3</v>
       </c>
@@ -35990,7 +36002,7 @@
         <v>-2.6329999999999999E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:37">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>-5.1079999999999997E-3</v>
       </c>
@@ -36103,7 +36115,7 @@
         <v>-2.967E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:37">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>-3.8509999999999998E-3</v>
       </c>
@@ -36216,7 +36228,7 @@
         <v>-2.0950000000000001E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:37">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>-1.008E-3</v>
       </c>
@@ -36329,7 +36341,7 @@
         <v>-4.5399999999999998E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:37">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2.6949999999999999E-3</v>
       </c>
@@ -36442,7 +36454,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:37">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>5.9519999999999998E-3</v>
       </c>
@@ -36555,7 +36567,7 @@
         <v>3.0739999999999999E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:37">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>7.9100000000000004E-3</v>
       </c>
@@ -36668,7 +36680,7 @@
         <v>3.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:37">
+    <row r="139" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>7.7559999999999999E-3</v>
       </c>
@@ -36781,7 +36793,7 @@
         <v>3.5839999999999999E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:37">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6.0660000000000002E-3</v>
       </c>
@@ -36894,7 +36906,7 @@
         <v>2.3960000000000001E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:37">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>3.14E-3</v>
       </c>
@@ -37007,7 +37019,7 @@
         <v>6.3100000000000005E-4</v>
       </c>
     </row>
-    <row r="142" spans="1:37">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>1.3200000000000001E-4</v>
       </c>
@@ -37120,7 +37132,7 @@
         <v>-1.075E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:37">
+    <row r="143" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>-2.2959999999999999E-3</v>
       </c>
@@ -37233,7 +37245,7 @@
         <v>-2.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:37">
+    <row r="144" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>-3.689E-3</v>
       </c>
@@ -37346,7 +37358,7 @@
         <v>-2.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:37">
+    <row r="145" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>-3.5109999999999998E-3</v>
       </c>
@@ -37459,7 +37471,7 @@
         <v>-2.5010000000000002E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:37">
+    <row r="146" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>-1.6869999999999999E-3</v>
       </c>
@@ -37572,7 +37584,7 @@
         <v>-1.4090000000000001E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:37">
+    <row r="147" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>9.01E-4</v>
       </c>
@@ -37685,7 +37697,7 @@
         <v>3.4999999999999997E-5</v>
       </c>
     </row>
-    <row r="148" spans="1:37">
+    <row r="148" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>3.9820000000000003E-3</v>
       </c>
@@ -37798,7 +37810,7 @@
         <v>1.7949999999999999E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:37">
+    <row r="149" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>7.1980000000000004E-3</v>
       </c>
@@ -37911,7 +37923,7 @@
         <v>3.2130000000000001E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:37">
+    <row r="150" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>8.8610000000000008E-3</v>
       </c>
@@ -38024,7 +38036,7 @@
         <v>4.1510000000000002E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:37">
+    <row r="151" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1.0116999999999999E-2</v>
       </c>
@@ -38137,7 +38149,7 @@
         <v>4.3810000000000003E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:37">
+    <row r="152" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>9.9889999999999996E-3</v>
       </c>
@@ -38250,7 +38262,7 @@
         <v>4.0749999999999996E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:37">
+    <row r="153" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>8.7559999999999999E-3</v>
       </c>
@@ -38363,7 +38375,7 @@
         <v>3.13E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:37">
+    <row r="154" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>7.2090000000000001E-3</v>
       </c>
@@ -38476,7 +38488,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:37">
+    <row r="155" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>4.4799999999999996E-3</v>
       </c>
@@ -38589,7 +38601,7 @@
         <v>3.3500000000000001E-4</v>
       </c>
     </row>
-    <row r="156" spans="1:37">
+    <row r="156" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1.864E-3</v>
       </c>
@@ -38702,7 +38714,7 @@
         <v>-9.5600000000000004E-4</v>
       </c>
     </row>
-    <row r="157" spans="1:37">
+    <row r="157" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2.3699999999999999E-4</v>
       </c>
@@ -38815,7 +38827,7 @@
         <v>-1.952E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:37">
+    <row r="158" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>-1.8400000000000001E-3</v>
       </c>
@@ -38928,7 +38940,7 @@
         <v>-2.8530000000000001E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:37">
+    <row r="159" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>-2.4559999999999998E-3</v>
       </c>
@@ -39041,7 +39053,7 @@
         <v>-3.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:37">
+    <row r="160" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>-2.1870000000000001E-3</v>
       </c>
@@ -39154,7 +39166,7 @@
         <v>-3.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:37">
+    <row r="161" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>-2.7109999999999999E-3</v>
       </c>

</xml_diff>

<commit_message>
CP01CNSP Cal and Ingest Sheet Check
Made corrections to Cal and Ingest sheet
</commit_message>
<xml_diff>
--- a/CP01CNSP/Omaha_Cal_Info_CP01CNSP_00004.xlsx
+++ b/CP01CNSP/Omaha_Cal_Info_CP01CNSP_00004.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\CP01CNSP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="5895" windowWidth="29040" windowHeight="13800" tabRatio="579" activeTab="1"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
     <definedName name="acs_181_calData" localSheetId="4">Sheet1!$A$1:$CA$161</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2326,7 +2331,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2399,9 @@
       <c r="D2" s="37">
         <v>42208</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="38">
+        <v>6.25E-2</v>
+      </c>
       <c r="F2" s="30"/>
       <c r="G2" s="43" t="s">
         <v>101</v>
@@ -2411,8 +2418,14 @@
       <c r="K2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="L2" s="16">
+        <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
+        <v>40.134166666666665</v>
+      </c>
+      <c r="M2" s="16">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
+        <v>-70.77</v>
+      </c>
     </row>
     <row r="3" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C3" s="22"/>
@@ -2519,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>